<commit_message>
updated data file winter 2022
updated with game schedule
</commit_message>
<xml_diff>
--- a/data/2022Winter_DraftedTeams_Emails_Website.xlsx
+++ b/data/2022Winter_DraftedTeams_Emails_Website.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pdwalker\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2EFBBB-ED01-4081-A09E-8A3344A7FAB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C03FEFD-ED2E-4F10-97AC-A40EF489A426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31155" yWindow="435" windowWidth="25575" windowHeight="14415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2700" yWindow="630" windowWidth="25575" windowHeight="14760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="gamesched" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$G$76</definedName>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1334" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="345">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1012,12 +1013,63 @@
   </si>
   <si>
     <t>Carolyn Godwin</t>
+  </si>
+  <si>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>Game</t>
+  </si>
+  <si>
+    <t>Field 1</t>
+  </si>
+  <si>
+    <t>Field 2</t>
+  </si>
+  <si>
+    <t>Counts</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>M vs PM</t>
+  </si>
+  <si>
+    <t>JL vs SC</t>
+  </si>
+  <si>
+    <t>Regular</t>
+  </si>
+  <si>
+    <t>M vs JL</t>
+  </si>
+  <si>
+    <t>PM vs SC</t>
+  </si>
+  <si>
+    <t>M vs SC</t>
+  </si>
+  <si>
+    <t>PM vs JL</t>
+  </si>
+  <si>
+    <t>Tourney</t>
+  </si>
+  <si>
+    <t>TBD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mmm\ d"/>
+  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1107,7 +1159,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1125,6 +1177,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5274,7 +5330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2BD999F-A439-411E-8987-30909891D5D5}">
   <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -7059,4 +7115,515 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC042FE7-DD2C-4227-BB73-8C720EB7799C}">
+  <dimension ref="A1:L20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:L20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>330</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>332</v>
+      </c>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>333</v>
+      </c>
+      <c r="I1" s="17"/>
+      <c r="J1" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>334</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="18">
+        <v>1</v>
+      </c>
+      <c r="B2" s="18">
+        <v>1</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="H2" s="19">
+        <v>6</v>
+      </c>
+      <c r="I2" s="17"/>
+      <c r="J2" s="18">
+        <v>1</v>
+      </c>
+      <c r="K2" s="20">
+        <v>44569</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="18">
+        <v>1</v>
+      </c>
+      <c r="B3" s="18">
+        <v>2</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>340</v>
+      </c>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="H3" s="19">
+        <v>5</v>
+      </c>
+      <c r="I3" s="17"/>
+      <c r="J3" s="18">
+        <v>2</v>
+      </c>
+      <c r="K3" s="20">
+        <v>44576</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="18">
+        <v>2</v>
+      </c>
+      <c r="B4" s="18">
+        <v>1</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>341</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="18" t="s">
+        <v>341</v>
+      </c>
+      <c r="H4" s="19">
+        <v>5</v>
+      </c>
+      <c r="I4" s="17"/>
+      <c r="J4" s="18">
+        <v>3</v>
+      </c>
+      <c r="K4" s="20">
+        <v>44583</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="18">
+        <v>2</v>
+      </c>
+      <c r="B5" s="18">
+        <v>2</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="H5" s="19">
+        <v>6</v>
+      </c>
+      <c r="I5" s="17"/>
+      <c r="J5" s="18">
+        <v>4</v>
+      </c>
+      <c r="K5" s="20">
+        <v>44590</v>
+      </c>
+      <c r="L5" s="18" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="18">
+        <v>3</v>
+      </c>
+      <c r="B6" s="18">
+        <v>1</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>340</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="18" t="s">
+        <v>340</v>
+      </c>
+      <c r="H6" s="19">
+        <v>5</v>
+      </c>
+      <c r="I6" s="17"/>
+      <c r="J6" s="18">
+        <v>5</v>
+      </c>
+      <c r="K6" s="20">
+        <v>44597</v>
+      </c>
+      <c r="L6" s="18" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="18">
+        <v>3</v>
+      </c>
+      <c r="B7" s="18">
+        <v>2</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>341</v>
+      </c>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="H7" s="19">
+        <v>5</v>
+      </c>
+      <c r="I7" s="17"/>
+      <c r="J7" s="18">
+        <v>6</v>
+      </c>
+      <c r="K7" s="20">
+        <v>44604</v>
+      </c>
+      <c r="L7" s="18" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="18">
+        <v>4</v>
+      </c>
+      <c r="B8" s="18">
+        <v>1</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="18">
+        <v>7</v>
+      </c>
+      <c r="K8" s="20">
+        <v>44611</v>
+      </c>
+      <c r="L8" s="18" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="18">
+        <v>4</v>
+      </c>
+      <c r="B9" s="18">
+        <v>2</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>340</v>
+      </c>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="18">
+        <v>8</v>
+      </c>
+      <c r="K9" s="20">
+        <v>44618</v>
+      </c>
+      <c r="L9" s="18" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="18">
+        <v>5</v>
+      </c>
+      <c r="B10" s="18">
+        <v>1</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>341</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="18">
+        <v>9</v>
+      </c>
+      <c r="K10" s="20">
+        <v>44625</v>
+      </c>
+      <c r="L10" s="18" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="18">
+        <v>5</v>
+      </c>
+      <c r="B11" s="18">
+        <v>2</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="18">
+        <v>6</v>
+      </c>
+      <c r="B12" s="18">
+        <v>1</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>340</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="18">
+        <v>6</v>
+      </c>
+      <c r="B13" s="18">
+        <v>2</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>341</v>
+      </c>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="18">
+        <v>7</v>
+      </c>
+      <c r="B14" s="18">
+        <v>1</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="18">
+        <v>7</v>
+      </c>
+      <c r="B15" s="18">
+        <v>2</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>340</v>
+      </c>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="18">
+        <v>8</v>
+      </c>
+      <c r="B16" s="18">
+        <v>1</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>341</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="18">
+        <v>8</v>
+      </c>
+      <c r="B17" s="18">
+        <v>2</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="18">
+        <v>9</v>
+      </c>
+      <c r="B18" s="18">
+        <v>1</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>344</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="18">
+        <v>9</v>
+      </c>
+      <c r="B19" s="18">
+        <v>2</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>344</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="18">
+        <v>9</v>
+      </c>
+      <c r="B20" s="18">
+        <v>3</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>344</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>344</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>